<commit_message>
averages instead of median in the table (discuss)
</commit_message>
<xml_diff>
--- a/rq1/avgs.xlsx
+++ b/rq1/avgs.xlsx
@@ -339,7 +339,7 @@
   <dimension ref="A1:X11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+      <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -719,10 +719,18 @@
         <f>AVERAGE(A1:X1)</f>
         <v>2.5</v>
       </c>
+      <c r="L7">
+        <f>AVERAGE(D1:F1)</f>
+        <v>1.6666666666666667</v>
+      </c>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.3">
       <c r="C8">
         <f t="shared" ref="C8:C11" si="0">AVERAGE(A2:X2)</f>
+        <v>1</v>
+      </c>
+      <c r="L8">
+        <f t="shared" ref="L8:L11" si="1">AVERAGE(D2:F2)</f>
         <v>1</v>
       </c>
     </row>
@@ -731,6 +739,10 @@
         <f t="shared" si="0"/>
         <v>0.875</v>
       </c>
+      <c r="L9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.3">
       <c r="C10">
@@ -745,6 +757,10 @@
         <f>COUNTIF(A4:X4,0)</f>
         <v>11</v>
       </c>
+      <c r="L10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.3">
       <c r="C11">
@@ -755,6 +771,10 @@
         <f>AVERAGEIF(A5:X5, "&gt;0")</f>
         <v>1.6</v>
       </c>
+      <c r="L11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
amend results in thesis and re-examine
</commit_message>
<xml_diff>
--- a/rq1/avgs.xlsx
+++ b/rq1/avgs.xlsx
@@ -23,9 +23,23 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+  <si>
+    <t>cm</t>
+  </si>
+  <si>
+    <t>pm</t>
+  </si>
+  <si>
+    <t>pf</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -33,13 +47,49 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -51,13 +101,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="4">
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -338,8 +397,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -363,31 +422,31 @@
       <c r="F1">
         <v>1</v>
       </c>
-      <c r="G1">
-        <v>3</v>
-      </c>
-      <c r="H1">
-        <v>3</v>
-      </c>
-      <c r="I1">
-        <v>3</v>
-      </c>
-      <c r="J1">
-        <v>1</v>
-      </c>
-      <c r="K1">
-        <v>1</v>
-      </c>
-      <c r="L1">
-        <v>1</v>
-      </c>
-      <c r="M1">
-        <v>3</v>
-      </c>
-      <c r="N1">
-        <v>3</v>
-      </c>
-      <c r="O1">
+      <c r="G1" s="2">
+        <v>2</v>
+      </c>
+      <c r="H1" s="2">
+        <v>3</v>
+      </c>
+      <c r="I1" s="2">
+        <v>1</v>
+      </c>
+      <c r="J1" s="3">
+        <v>1</v>
+      </c>
+      <c r="K1" s="3">
+        <v>1</v>
+      </c>
+      <c r="L1" s="3">
+        <v>1</v>
+      </c>
+      <c r="M1" s="1">
+        <v>3</v>
+      </c>
+      <c r="N1" s="1">
+        <v>3</v>
+      </c>
+      <c r="O1" s="1">
         <v>3</v>
       </c>
       <c r="P1">
@@ -437,31 +496,31 @@
       <c r="F2">
         <v>1</v>
       </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2">
-        <v>1</v>
-      </c>
-      <c r="I2">
-        <v>1</v>
-      </c>
-      <c r="J2">
-        <v>1</v>
-      </c>
-      <c r="K2">
-        <v>1</v>
-      </c>
-      <c r="L2">
-        <v>1</v>
-      </c>
-      <c r="M2">
-        <v>1</v>
-      </c>
-      <c r="N2">
-        <v>1</v>
-      </c>
-      <c r="O2">
+      <c r="G2" s="2">
+        <v>1</v>
+      </c>
+      <c r="H2" s="2">
+        <v>1</v>
+      </c>
+      <c r="I2" s="2">
+        <v>1</v>
+      </c>
+      <c r="J2" s="3">
+        <v>1</v>
+      </c>
+      <c r="K2" s="3">
+        <v>1</v>
+      </c>
+      <c r="L2" s="3">
+        <v>1</v>
+      </c>
+      <c r="M2" s="1">
+        <v>1</v>
+      </c>
+      <c r="N2" s="1">
+        <v>1</v>
+      </c>
+      <c r="O2" s="1">
         <v>1</v>
       </c>
       <c r="P2">
@@ -511,32 +570,32 @@
       <c r="F3">
         <v>0</v>
       </c>
-      <c r="G3">
-        <v>1</v>
-      </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
-      <c r="I3">
-        <v>1</v>
-      </c>
-      <c r="J3">
-        <v>2</v>
-      </c>
-      <c r="K3">
-        <v>2</v>
-      </c>
-      <c r="L3">
-        <v>2</v>
-      </c>
-      <c r="M3">
-        <v>2</v>
-      </c>
-      <c r="N3">
-        <v>0</v>
-      </c>
-      <c r="O3">
-        <v>1</v>
+      <c r="G3" s="2">
+        <v>2</v>
+      </c>
+      <c r="H3" s="2">
+        <v>0</v>
+      </c>
+      <c r="I3" s="2">
+        <v>2</v>
+      </c>
+      <c r="J3" s="3">
+        <v>2</v>
+      </c>
+      <c r="K3" s="3">
+        <v>2</v>
+      </c>
+      <c r="L3" s="3">
+        <v>2</v>
+      </c>
+      <c r="M3" s="1">
+        <v>2</v>
+      </c>
+      <c r="N3" s="1">
+        <v>2</v>
+      </c>
+      <c r="O3" s="1">
+        <v>2</v>
       </c>
       <c r="P3">
         <v>1</v>
@@ -585,32 +644,32 @@
       <c r="F4">
         <v>0</v>
       </c>
-      <c r="G4">
-        <v>3</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-      <c r="I4">
-        <v>3</v>
-      </c>
-      <c r="J4">
-        <v>3</v>
-      </c>
-      <c r="K4">
-        <v>3</v>
-      </c>
-      <c r="L4">
-        <v>1</v>
-      </c>
-      <c r="M4">
-        <v>3</v>
-      </c>
-      <c r="N4">
-        <v>0</v>
-      </c>
-      <c r="O4">
-        <v>2</v>
+      <c r="G4" s="2">
+        <v>3</v>
+      </c>
+      <c r="H4" s="2">
+        <v>0</v>
+      </c>
+      <c r="I4" s="2">
+        <v>0</v>
+      </c>
+      <c r="J4" s="3">
+        <v>3</v>
+      </c>
+      <c r="K4" s="3">
+        <v>3</v>
+      </c>
+      <c r="L4" s="3">
+        <v>3</v>
+      </c>
+      <c r="M4" s="1">
+        <v>3</v>
+      </c>
+      <c r="N4" s="1">
+        <v>3</v>
+      </c>
+      <c r="O4" s="1">
+        <v>3</v>
       </c>
       <c r="P4">
         <v>3</v>
@@ -659,32 +718,32 @@
       <c r="F5">
         <v>0</v>
       </c>
-      <c r="G5">
-        <v>3</v>
-      </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
-      <c r="I5">
-        <v>3</v>
-      </c>
-      <c r="J5">
-        <v>1</v>
-      </c>
-      <c r="K5">
-        <v>1</v>
-      </c>
-      <c r="L5">
-        <v>0</v>
-      </c>
-      <c r="M5">
-        <v>0</v>
-      </c>
-      <c r="N5">
-        <v>0</v>
-      </c>
-      <c r="O5">
-        <v>2</v>
+      <c r="G5" s="2">
+        <v>1</v>
+      </c>
+      <c r="H5" s="2">
+        <v>0</v>
+      </c>
+      <c r="I5" s="2">
+        <v>0</v>
+      </c>
+      <c r="J5" s="3">
+        <v>1</v>
+      </c>
+      <c r="K5" s="3">
+        <v>1</v>
+      </c>
+      <c r="L5" s="3">
+        <v>3</v>
+      </c>
+      <c r="M5" s="1">
+        <v>3</v>
+      </c>
+      <c r="N5" s="1">
+        <v>2</v>
+      </c>
+      <c r="O5" s="1">
+        <v>3</v>
       </c>
       <c r="P5">
         <v>0</v>
@@ -711,13 +770,24 @@
         <v>2</v>
       </c>
       <c r="X5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="H6" t="s">
+        <v>1</v>
+      </c>
+      <c r="K6" t="s">
+        <v>2</v>
+      </c>
+      <c r="N6" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.3">
       <c r="C7">
         <f>AVERAGE(A1:X1)</f>
-        <v>2.5</v>
+        <v>2.375</v>
       </c>
       <c r="L7">
         <f>AVERAGE(D1:F1)</f>
@@ -737,7 +807,7 @@
     <row r="9" spans="1:24" x14ac:dyDescent="0.3">
       <c r="C9">
         <f t="shared" si="0"/>
-        <v>0.875</v>
+        <v>1.0833333333333333</v>
       </c>
       <c r="L9">
         <f t="shared" si="1"/>
@@ -747,11 +817,11 @@
     <row r="10" spans="1:24" x14ac:dyDescent="0.3">
       <c r="C10">
         <f t="shared" si="0"/>
-        <v>1.5</v>
+        <v>1.625</v>
       </c>
       <c r="D10">
         <f>AVERAGEIF(A4:X4, "&gt;0")</f>
-        <v>2.7692307692307692</v>
+        <v>3</v>
       </c>
       <c r="E10">
         <f>COUNTIF(A4:X4,0)</f>
@@ -765,11 +835,11 @@
     <row r="11" spans="1:24" x14ac:dyDescent="0.3">
       <c r="C11">
         <f t="shared" si="0"/>
-        <v>0.66666666666666663</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="D11">
         <f>AVERAGEIF(A5:X5, "&gt;0")</f>
-        <v>1.6</v>
+        <v>1.6666666666666667</v>
       </c>
       <c r="L11">
         <f t="shared" si="1"/>

</xml_diff>